<commit_message>
Java Program to Read files and Creating Database Tables according to that
</commit_message>
<xml_diff>
--- a/src/main/resource/kenit.xlsx
+++ b/src/main/resource/kenit.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenit\eclipse-workspace\Importer\src\main\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenit\Desktop\Git Repo\ExcelImporter\src\main\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA67D862-09CF-40E3-BC2A-B909A25A3ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC12F844-3C17-487D-99B9-9F3D936BD738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F58983CE-F7EF-488B-B80A-DE79792F27E6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F58983CE-F7EF-488B-B80A-DE79792F27E6}"/>
   </bookViews>
   <sheets>
     <sheet name="kenit" sheetId="1" r:id="rId1"/>
-    <sheet name="nirali" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="mkm">kenit!$A:$A</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -53,48 +55,6 @@
   </si>
   <si>
     <t>6'5</t>
-  </si>
-  <si>
-    <t>no.</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>salary</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Kunal</t>
-  </si>
-  <si>
-    <t>Sumeet</t>
-  </si>
-  <si>
-    <t>Kishan</t>
-  </si>
-  <si>
-    <t>Harshil</t>
-  </si>
-  <si>
-    <t>Haard</t>
-  </si>
-  <si>
-    <t>Jainam</t>
-  </si>
-  <si>
-    <t>Jash</t>
-  </si>
-  <si>
-    <t>eng</t>
   </si>
 </sst>
 </file>
@@ -448,9 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAFA8D22-A449-4568-A926-50C7CDE60D5C}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -501,206 +459,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C05A160-7976-4012-AA9F-F39A10CC5456}">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>98989898</v>
-      </c>
-      <c r="D2">
-        <v>10000</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>98989898</v>
-      </c>
-      <c r="D3">
-        <v>1000</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4">
-        <v>98989898</v>
-      </c>
-      <c r="D4">
-        <v>100000</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5">
-        <v>98989898</v>
-      </c>
-      <c r="D5">
-        <v>100000</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>98989898</v>
-      </c>
-      <c r="D6">
-        <v>100</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>98989898</v>
-      </c>
-      <c r="D7">
-        <v>10000</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>98989898</v>
-      </c>
-      <c r="D8">
-        <v>10000</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9">
-        <v>98989898</v>
-      </c>
-      <c r="D9">
-        <v>100000</v>
-      </c>
-      <c r="E9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10">
-        <v>98989898</v>
-      </c>
-      <c r="D10">
-        <v>100000</v>
-      </c>
-      <c r="E10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11">
-        <v>98989898</v>
-      </c>
-      <c r="D11">
-        <v>10000</v>
-      </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>